<commit_message>
change patch version names to Manual and Auto
</commit_message>
<xml_diff>
--- a/1. D4J_Correct_NoDupl_Metrics/Defects4J_Correct_Project_67_BasicInfo_Avg.xlsx
+++ b/1. D4J_Correct_NoDupl_Metrics/Defects4J_Correct_Project_67_BasicInfo_Avg.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UROS\Desktop\VM Shared Folder\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UROS\Documents\GitHub\APR-PQA\1. D4J_Correct_NoDupl_Metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -578,27 +578,9 @@
     <t>NbMethodsCallingMe</t>
   </si>
   <si>
-    <t>Lang-51-Repaired</t>
-  </si>
-  <si>
-    <t>Math-34-Fixed</t>
-  </si>
-  <si>
-    <t>Lang-43-Fixed</t>
-  </si>
-  <si>
-    <t>Mockito-22-Fixed</t>
-  </si>
-  <si>
-    <t>Closure-86-Fixed</t>
-  </si>
-  <si>
     <t>Closure-6-Buggy</t>
   </si>
   <si>
-    <t>Chart-12-Fixed</t>
-  </si>
-  <si>
     <t>Math-3-Buggy</t>
   </si>
   <si>
@@ -608,45 +590,18 @@
     <t>Closure-15-Buggy</t>
   </si>
   <si>
-    <t>Math-59-Repaired</t>
-  </si>
-  <si>
-    <t>Math-61-Repaired</t>
-  </si>
-  <si>
     <t>Math-79-Buggy</t>
   </si>
   <si>
     <t>Math-82-Buggy</t>
   </si>
   <si>
-    <t>Chart-26-Repaired</t>
-  </si>
-  <si>
     <t>Chart-14-Buggy</t>
   </si>
   <si>
-    <t>Closure-70-Repaired</t>
-  </si>
-  <si>
-    <t>Closure-6-Fixed</t>
-  </si>
-  <si>
-    <t>Math-41-Fixed</t>
-  </si>
-  <si>
     <t>Math-30-Buggy</t>
   </si>
   <si>
-    <t>Closure-78-Repaired</t>
-  </si>
-  <si>
-    <t>Math-85-Fixed</t>
-  </si>
-  <si>
-    <t>Math-57-Repaired</t>
-  </si>
-  <si>
     <t>Mockito-22-Buggy</t>
   </si>
   <si>
@@ -656,159 +611,51 @@
     <t>Math-53-Buggy</t>
   </si>
   <si>
-    <t>Lang-55-Fixed</t>
-  </si>
-  <si>
-    <t>Chart-9-Repaired</t>
-  </si>
-  <si>
-    <t>Math-57-Fixed</t>
-  </si>
-  <si>
     <t>Lang-55-Buggy</t>
   </si>
   <si>
-    <t>Closure-38-Fixed</t>
-  </si>
-  <si>
     <t>Closure-123-Buggy</t>
   </si>
   <si>
-    <t>Math-69-Fixed</t>
-  </si>
-  <si>
-    <t>Closure-123-Fixed</t>
-  </si>
-  <si>
-    <t>Math-30-Fixed</t>
-  </si>
-  <si>
     <t>Lang-29-Buggy</t>
   </si>
   <si>
-    <t>Lang-10-Fixed</t>
-  </si>
-  <si>
-    <t>Math-69-Repaired</t>
-  </si>
-  <si>
     <t>Math-58-Buggy</t>
   </si>
   <si>
-    <t>Closure-18-Fixed</t>
-  </si>
-  <si>
-    <t>Lang-21-Fixed</t>
-  </si>
-  <si>
-    <t>Time-15-Fixed</t>
-  </si>
-  <si>
-    <t>Time-19-Repaired</t>
-  </si>
-  <si>
     <t>Math-27-Buggy</t>
   </si>
   <si>
     <t>Lang-44-Buggy</t>
   </si>
   <si>
-    <t>Lang-29-Repaired</t>
-  </si>
-  <si>
-    <t>Closure-18-Repaired</t>
-  </si>
-  <si>
-    <t>Mockito-22-Repaired</t>
-  </si>
-  <si>
     <t>Chart-12-Buggy</t>
   </si>
   <si>
     <t>Chart-7-Buggy</t>
   </si>
   <si>
-    <t>Closure-15-Fixed</t>
-  </si>
-  <si>
     <t>Math-65-Buggy</t>
   </si>
   <si>
-    <t>Closure-1-Fixed</t>
-  </si>
-  <si>
-    <t>Math-27-Fixed</t>
-  </si>
-  <si>
-    <t>Math-82-Repaired</t>
-  </si>
-  <si>
-    <t>Closure-68-Fixed</t>
-  </si>
-  <si>
-    <t>Mockito-29-Repaired</t>
-  </si>
-  <si>
-    <t>Lang-52-Fixed</t>
-  </si>
-  <si>
-    <t>Closure-4-Repaired</t>
-  </si>
-  <si>
-    <t>Closure-62-Repaired</t>
-  </si>
-  <si>
-    <t>Closure-119-Repaired</t>
-  </si>
-  <si>
-    <t>Time-19-Fixed</t>
-  </si>
-  <si>
-    <t>Lang-43-Repaired</t>
-  </si>
-  <si>
-    <t>Math-27-Repaired</t>
-  </si>
-  <si>
     <t>Math-25-Buggy</t>
   </si>
   <si>
-    <t>Mockito-29-Fixed</t>
-  </si>
-  <si>
-    <t>Chart-9-Fixed</t>
-  </si>
-  <si>
     <t>Closure-1-Buggy</t>
   </si>
   <si>
-    <t>Closure-115-Repaired</t>
-  </si>
-  <si>
     <t>Closure-78-Buggy</t>
   </si>
   <si>
-    <t>Time-26-Repaired</t>
-  </si>
-  <si>
     <t>Closure-86-Buggy</t>
   </si>
   <si>
-    <t>Closure-6-Repaired</t>
-  </si>
-  <si>
     <t>Closure-4-Buggy</t>
   </si>
   <si>
     <t>Math-41-Buggy</t>
   </si>
   <si>
-    <t>Lang-35-Fixed</t>
-  </si>
-  <si>
-    <t>Closure-1-Repaired</t>
-  </si>
-  <si>
     <t>Math-69-Buggy</t>
   </si>
   <si>
@@ -818,102 +665,33 @@
     <t>Math-57-Buggy</t>
   </si>
   <si>
-    <t>Lang-51-Fixed</t>
-  </si>
-  <si>
-    <t>Closure-86-Repaired</t>
-  </si>
-  <si>
     <t>Math-61-Buggy</t>
   </si>
   <si>
-    <t>Chart-11-Fixed</t>
-  </si>
-  <si>
-    <t>Closure-118-Fixed</t>
-  </si>
-  <si>
-    <t>Lang-45-Fixed</t>
-  </si>
-  <si>
     <t>Closure-10-Buggy</t>
   </si>
   <si>
-    <t>Math-82-Fixed</t>
-  </si>
-  <si>
-    <t>Math-85-Repaired</t>
-  </si>
-  <si>
-    <t>Math-70-Fixed</t>
-  </si>
-  <si>
     <t>Closure-68-Buggy</t>
   </si>
   <si>
     <t>Lang-49-Buggy</t>
   </si>
   <si>
-    <t>Math-79-Fixed</t>
-  </si>
-  <si>
-    <t>Math-53-Fixed</t>
-  </si>
-  <si>
-    <t>Lang-45-Repaired</t>
-  </si>
-  <si>
-    <t>Closure-92-Repaired</t>
-  </si>
-  <si>
-    <t>Chart-14-Fixed</t>
-  </si>
-  <si>
     <t>Mockito-29-Buggy</t>
   </si>
   <si>
-    <t>Closure-78-Fixed</t>
-  </si>
-  <si>
     <t>Lang-6-Buggy</t>
   </si>
   <si>
-    <t>Math-3-Fixed</t>
-  </si>
-  <si>
-    <t>Lang-10-Repaired</t>
-  </si>
-  <si>
-    <t>Math-25-Repaired</t>
-  </si>
-  <si>
-    <t>Math-58-Fixed</t>
-  </si>
-  <si>
-    <t>Math-50-Fixed</t>
-  </si>
-  <si>
     <t>Lang-43-Buggy</t>
   </si>
   <si>
     <t>Math-34-Buggy</t>
   </si>
   <si>
-    <t>Chart-12-Repaired</t>
-  </si>
-  <si>
     <t>Closure-46-Buggy</t>
   </si>
   <si>
-    <t>Chart-26-Fixed</t>
-  </si>
-  <si>
-    <t>Chart-14-Repaired</t>
-  </si>
-  <si>
-    <t>Lang-29-Fixed</t>
-  </si>
-  <si>
     <t>Closure-119-Buggy</t>
   </si>
   <si>
@@ -926,54 +704,21 @@
     <t>Closure-115-Buggy</t>
   </si>
   <si>
-    <t>Closure-92-Fixed</t>
-  </si>
-  <si>
     <t>Lang-58-Buggy</t>
   </si>
   <si>
-    <t>Closure-119-Fixed</t>
-  </si>
-  <si>
     <t>Lang-10-Buggy</t>
   </si>
   <si>
-    <t>Lang-49-Fixed</t>
-  </si>
-  <si>
-    <t>Math-30-Repaired</t>
-  </si>
-  <si>
-    <t>Math-11-Fixed</t>
-  </si>
-  <si>
     <t>Lang-35-Buggy</t>
   </si>
   <si>
     <t>Closure-40-Buggy</t>
   </si>
   <si>
-    <t>Chart-7-Repaired</t>
-  </si>
-  <si>
-    <t>Lang-55-Repaired</t>
-  </si>
-  <si>
-    <t>Math-65-Repaired</t>
-  </si>
-  <si>
-    <t>Closure-123-Repaired</t>
-  </si>
-  <si>
-    <t>Math-34-Repaired</t>
-  </si>
-  <si>
     <t>Math-56-Buggy</t>
   </si>
   <si>
-    <t>Math-80-Repaired</t>
-  </si>
-  <si>
     <t>Math-85-Buggy</t>
   </si>
   <si>
@@ -983,69 +728,18 @@
     <t>Math-59-Buggy</t>
   </si>
   <si>
-    <t>Math-70-Repaired</t>
-  </si>
-  <si>
     <t>Lang-45-Buggy</t>
   </si>
   <si>
     <t>Math-50-Buggy</t>
   </si>
   <si>
-    <t>Chart-11-Repaired</t>
-  </si>
-  <si>
-    <t>Lang-49-Repaired</t>
-  </si>
-  <si>
-    <t>Math-33-Fixed</t>
-  </si>
-  <si>
-    <t>Math-65-Fixed</t>
-  </si>
-  <si>
-    <t>Closure-46-Repaired</t>
-  </si>
-  <si>
-    <t>Time-26-Fixed</t>
-  </si>
-  <si>
-    <t>Math-3-Repaired</t>
-  </si>
-  <si>
-    <t>Closure-4-Fixed</t>
-  </si>
-  <si>
-    <t>Lang-6-Fixed</t>
-  </si>
-  <si>
     <t>Time-15-Buggy</t>
   </si>
   <si>
-    <t>Closure-38-Repaired</t>
-  </si>
-  <si>
-    <t>Lang-21-Repaired</t>
-  </si>
-  <si>
-    <t>Closure-10-Fixed</t>
-  </si>
-  <si>
-    <t>Lang-35-Repaired</t>
-  </si>
-  <si>
-    <t>Math-56-Fixed</t>
-  </si>
-  <si>
     <t>Math-33-Buggy</t>
   </si>
   <si>
-    <t>Closure-62-Fixed</t>
-  </si>
-  <si>
-    <t>Time-15-Repaired</t>
-  </si>
-  <si>
     <t>Chart-9-Buggy</t>
   </si>
   <si>
@@ -1055,72 +749,18 @@
     <t>Closure-38-Buggy</t>
   </si>
   <si>
-    <t>Lang-44-Fixed</t>
-  </si>
-  <si>
     <t>Closure-18-Buggy</t>
   </si>
   <si>
-    <t>Math-41-Repaired</t>
-  </si>
-  <si>
     <t>Chart-26-Buggy</t>
   </si>
   <si>
-    <t>Closure-40-Fixed</t>
-  </si>
-  <si>
-    <t>Closure-15-Repaired</t>
-  </si>
-  <si>
-    <t>Lang-44-Repaired</t>
-  </si>
-  <si>
-    <t>Math-50-Repaired</t>
-  </si>
-  <si>
-    <t>Math-11-Repaired</t>
-  </si>
-  <si>
-    <t>Closure-115-Fixed</t>
-  </si>
-  <si>
-    <t>Math-79-Repaired</t>
-  </si>
-  <si>
-    <t>Math-25-Fixed</t>
-  </si>
-  <si>
-    <t>Lang-58-Fixed</t>
-  </si>
-  <si>
-    <t>Math-53-Repaired</t>
-  </si>
-  <si>
-    <t>Math-75-Fixed</t>
-  </si>
-  <si>
-    <t>Math-80-Fixed</t>
-  </si>
-  <si>
     <t>Closure-92-Buggy</t>
   </si>
   <si>
-    <t>Closure-118-Repaired</t>
-  </si>
-  <si>
-    <t>Closure-40-Repaired</t>
-  </si>
-  <si>
     <t>Math-5-Buggy</t>
   </si>
   <si>
-    <t>Math-5-Repaired</t>
-  </si>
-  <si>
-    <t>Math-5-Fixed</t>
-  </si>
-  <si>
     <t>Math-75-Buggy</t>
   </si>
   <si>
@@ -1130,57 +770,15 @@
     <t>Time-26-Buggy</t>
   </si>
   <si>
-    <t>Math-75-Repaired</t>
-  </si>
-  <si>
-    <t>Closure-10-Repaired</t>
-  </si>
-  <si>
-    <t>Math-56-Repaired</t>
-  </si>
-  <si>
-    <t>Math-61-Fixed</t>
-  </si>
-  <si>
-    <t>Closure-68-Repaired</t>
-  </si>
-  <si>
-    <t>Math-59-Fixed</t>
-  </si>
-  <si>
-    <t>Closure-46-Fixed</t>
-  </si>
-  <si>
-    <t>Lang-58-Repaired</t>
-  </si>
-  <si>
     <t>Lang-52-Buggy</t>
   </si>
   <si>
-    <t>Lang-52-Repaired</t>
-  </si>
-  <si>
     <t>Math-70-Buggy</t>
   </si>
   <si>
-    <t>Chart-7-Fixed</t>
-  </si>
-  <si>
-    <t>Lang-6-Repaired</t>
-  </si>
-  <si>
-    <t>Math-33-Repaired</t>
-  </si>
-  <si>
     <t>Closure-62-Buggy</t>
   </si>
   <si>
-    <t>Math-58-Repaired</t>
-  </si>
-  <si>
-    <t>Closure-70-Fixed</t>
-  </si>
-  <si>
     <t>Sum:</t>
   </si>
   <si>
@@ -1200,6 +798,408 @@
   </si>
   <si>
     <t>201 projects</t>
+  </si>
+  <si>
+    <t>Chart-11-Auto</t>
+  </si>
+  <si>
+    <t>Chart-12-Auto</t>
+  </si>
+  <si>
+    <t>Chart-14-Auto</t>
+  </si>
+  <si>
+    <t>Chart-26-Auto</t>
+  </si>
+  <si>
+    <t>Chart-7-Auto</t>
+  </si>
+  <si>
+    <t>Chart-9-Auto</t>
+  </si>
+  <si>
+    <t>Closure-10-Auto</t>
+  </si>
+  <si>
+    <t>Closure-115-Auto</t>
+  </si>
+  <si>
+    <t>Closure-118-Auto</t>
+  </si>
+  <si>
+    <t>Closure-119-Auto</t>
+  </si>
+  <si>
+    <t>Closure-123-Auto</t>
+  </si>
+  <si>
+    <t>Closure-15-Auto</t>
+  </si>
+  <si>
+    <t>Closure-18-Auto</t>
+  </si>
+  <si>
+    <t>Closure-1-Auto</t>
+  </si>
+  <si>
+    <t>Closure-38-Auto</t>
+  </si>
+  <si>
+    <t>Closure-40-Auto</t>
+  </si>
+  <si>
+    <t>Closure-46-Auto</t>
+  </si>
+  <si>
+    <t>Closure-4-Auto</t>
+  </si>
+  <si>
+    <t>Closure-62-Auto</t>
+  </si>
+  <si>
+    <t>Closure-68-Auto</t>
+  </si>
+  <si>
+    <t>Closure-6-Auto</t>
+  </si>
+  <si>
+    <t>Closure-70-Auto</t>
+  </si>
+  <si>
+    <t>Closure-78-Auto</t>
+  </si>
+  <si>
+    <t>Closure-86-Auto</t>
+  </si>
+  <si>
+    <t>Closure-92-Auto</t>
+  </si>
+  <si>
+    <t>Lang-10-Auto</t>
+  </si>
+  <si>
+    <t>Lang-21-Auto</t>
+  </si>
+  <si>
+    <t>Lang-29-Auto</t>
+  </si>
+  <si>
+    <t>Lang-35-Auto</t>
+  </si>
+  <si>
+    <t>Lang-43-Auto</t>
+  </si>
+  <si>
+    <t>Lang-44-Auto</t>
+  </si>
+  <si>
+    <t>Lang-45-Auto</t>
+  </si>
+  <si>
+    <t>Lang-49-Auto</t>
+  </si>
+  <si>
+    <t>Lang-51-Auto</t>
+  </si>
+  <si>
+    <t>Lang-52-Auto</t>
+  </si>
+  <si>
+    <t>Lang-55-Auto</t>
+  </si>
+  <si>
+    <t>Lang-58-Auto</t>
+  </si>
+  <si>
+    <t>Lang-6-Auto</t>
+  </si>
+  <si>
+    <t>Math-11-Auto</t>
+  </si>
+  <si>
+    <t>Math-25-Auto</t>
+  </si>
+  <si>
+    <t>Math-27-Auto</t>
+  </si>
+  <si>
+    <t>Math-30-Auto</t>
+  </si>
+  <si>
+    <t>Math-33-Auto</t>
+  </si>
+  <si>
+    <t>Math-34-Auto</t>
+  </si>
+  <si>
+    <t>Math-3-Auto</t>
+  </si>
+  <si>
+    <t>Math-41-Auto</t>
+  </si>
+  <si>
+    <t>Math-50-Auto</t>
+  </si>
+  <si>
+    <t>Math-53-Auto</t>
+  </si>
+  <si>
+    <t>Math-56-Auto</t>
+  </si>
+  <si>
+    <t>Math-57-Auto</t>
+  </si>
+  <si>
+    <t>Math-58-Auto</t>
+  </si>
+  <si>
+    <t>Math-59-Auto</t>
+  </si>
+  <si>
+    <t>Math-5-Auto</t>
+  </si>
+  <si>
+    <t>Math-61-Auto</t>
+  </si>
+  <si>
+    <t>Math-65-Auto</t>
+  </si>
+  <si>
+    <t>Math-69-Auto</t>
+  </si>
+  <si>
+    <t>Math-70-Auto</t>
+  </si>
+  <si>
+    <t>Math-75-Auto</t>
+  </si>
+  <si>
+    <t>Math-79-Auto</t>
+  </si>
+  <si>
+    <t>Math-80-Auto</t>
+  </si>
+  <si>
+    <t>Math-82-Auto</t>
+  </si>
+  <si>
+    <t>Math-85-Auto</t>
+  </si>
+  <si>
+    <t>Mockito-22-Auto</t>
+  </si>
+  <si>
+    <t>Mockito-29-Auto</t>
+  </si>
+  <si>
+    <t>Time-15-Auto</t>
+  </si>
+  <si>
+    <t>Time-19-Auto</t>
+  </si>
+  <si>
+    <t>Time-26-Auto</t>
+  </si>
+  <si>
+    <t>Chart-11-Manual</t>
+  </si>
+  <si>
+    <t>Chart-12-Manual</t>
+  </si>
+  <si>
+    <t>Chart-14-Manual</t>
+  </si>
+  <si>
+    <t>Chart-26-Manual</t>
+  </si>
+  <si>
+    <t>Chart-7-Manual</t>
+  </si>
+  <si>
+    <t>Chart-9-Manual</t>
+  </si>
+  <si>
+    <t>Closure-10-Manual</t>
+  </si>
+  <si>
+    <t>Closure-115-Manual</t>
+  </si>
+  <si>
+    <t>Closure-118-Manual</t>
+  </si>
+  <si>
+    <t>Closure-119-Manual</t>
+  </si>
+  <si>
+    <t>Closure-123-Manual</t>
+  </si>
+  <si>
+    <t>Closure-15-Manual</t>
+  </si>
+  <si>
+    <t>Closure-18-Manual</t>
+  </si>
+  <si>
+    <t>Closure-1-Manual</t>
+  </si>
+  <si>
+    <t>Closure-38-Manual</t>
+  </si>
+  <si>
+    <t>Closure-40-Manual</t>
+  </si>
+  <si>
+    <t>Closure-46-Manual</t>
+  </si>
+  <si>
+    <t>Closure-4-Manual</t>
+  </si>
+  <si>
+    <t>Closure-62-Manual</t>
+  </si>
+  <si>
+    <t>Closure-68-Manual</t>
+  </si>
+  <si>
+    <t>Closure-6-Manual</t>
+  </si>
+  <si>
+    <t>Closure-70-Manual</t>
+  </si>
+  <si>
+    <t>Closure-78-Manual</t>
+  </si>
+  <si>
+    <t>Closure-86-Manual</t>
+  </si>
+  <si>
+    <t>Closure-92-Manual</t>
+  </si>
+  <si>
+    <t>Lang-10-Manual</t>
+  </si>
+  <si>
+    <t>Lang-21-Manual</t>
+  </si>
+  <si>
+    <t>Lang-29-Manual</t>
+  </si>
+  <si>
+    <t>Lang-35-Manual</t>
+  </si>
+  <si>
+    <t>Lang-43-Manual</t>
+  </si>
+  <si>
+    <t>Lang-44-Manual</t>
+  </si>
+  <si>
+    <t>Lang-45-Manual</t>
+  </si>
+  <si>
+    <t>Lang-49-Manual</t>
+  </si>
+  <si>
+    <t>Lang-51-Manual</t>
+  </si>
+  <si>
+    <t>Lang-52-Manual</t>
+  </si>
+  <si>
+    <t>Lang-55-Manual</t>
+  </si>
+  <si>
+    <t>Lang-58-Manual</t>
+  </si>
+  <si>
+    <t>Lang-6-Manual</t>
+  </si>
+  <si>
+    <t>Math-11-Manual</t>
+  </si>
+  <si>
+    <t>Math-25-Manual</t>
+  </si>
+  <si>
+    <t>Math-27-Manual</t>
+  </si>
+  <si>
+    <t>Math-30-Manual</t>
+  </si>
+  <si>
+    <t>Math-33-Manual</t>
+  </si>
+  <si>
+    <t>Math-34-Manual</t>
+  </si>
+  <si>
+    <t>Math-3-Manual</t>
+  </si>
+  <si>
+    <t>Math-41-Manual</t>
+  </si>
+  <si>
+    <t>Math-50-Manual</t>
+  </si>
+  <si>
+    <t>Math-53-Manual</t>
+  </si>
+  <si>
+    <t>Math-56-Manual</t>
+  </si>
+  <si>
+    <t>Math-57-Manual</t>
+  </si>
+  <si>
+    <t>Math-58-Manual</t>
+  </si>
+  <si>
+    <t>Math-59-Manual</t>
+  </si>
+  <si>
+    <t>Math-5-Manual</t>
+  </si>
+  <si>
+    <t>Math-61-Manual</t>
+  </si>
+  <si>
+    <t>Math-65-Manual</t>
+  </si>
+  <si>
+    <t>Math-69-Manual</t>
+  </si>
+  <si>
+    <t>Math-70-Manual</t>
+  </si>
+  <si>
+    <t>Math-75-Manual</t>
+  </si>
+  <si>
+    <t>Math-79-Manual</t>
+  </si>
+  <si>
+    <t>Math-80-Manual</t>
+  </si>
+  <si>
+    <t>Math-82-Manual</t>
+  </si>
+  <si>
+    <t>Math-85-Manual</t>
+  </si>
+  <si>
+    <t>Mockito-22-Manual</t>
+  </si>
+  <si>
+    <t>Mockito-29-Manual</t>
+  </si>
+  <si>
+    <t>Time-15-Manual</t>
+  </si>
+  <si>
+    <t>Time-19-Manual</t>
+  </si>
+  <si>
+    <t>Time-26-Manual</t>
   </si>
 </sst>
 </file>
@@ -2326,7 +2326,7 @@
     </row>
     <row r="18" spans="1:27" ht="28.8" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
-        <v>230</v>
+        <v>96</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>15</v>
@@ -2369,7 +2369,7 @@
     </row>
     <row r="19" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
-        <v>136</v>
+        <v>62</v>
       </c>
       <c r="B19" s="8">
         <v>8.9</v>
@@ -2411,7 +2411,7 @@
     </row>
     <row r="20" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="B20" s="8">
         <v>8.2899999999999991</v>
@@ -2453,7 +2453,7 @@
     </row>
     <row r="21" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B21" s="6">
         <v>6.74</v>
@@ -2495,7 +2495,7 @@
     </row>
     <row r="22" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
-        <v>185</v>
+        <v>81</v>
       </c>
       <c r="B22" s="6">
         <v>4.75</v>
@@ -2537,7 +2537,7 @@
     </row>
     <row r="23" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="B23" s="6">
         <v>4.67</v>
@@ -2579,7 +2579,7 @@
     </row>
     <row r="24" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
-        <v>179</v>
+        <v>77</v>
       </c>
       <c r="B24" s="6">
         <v>5.75</v>
@@ -2622,7 +2622,7 @@
     </row>
     <row r="25" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
-        <v>109</v>
+        <v>53</v>
       </c>
       <c r="B25" s="8">
         <v>5.41</v>
@@ -2664,7 +2664,7 @@
     </row>
     <row r="26" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
-        <v>138</v>
+        <v>64</v>
       </c>
       <c r="B26" s="8">
         <v>10.33</v>
@@ -2706,7 +2706,7 @@
     </row>
     <row r="27" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
-        <v>156</v>
+        <v>71</v>
       </c>
       <c r="B27" s="8">
         <v>4.99</v>
@@ -2748,7 +2748,7 @@
     </row>
     <row r="28" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
-        <v>135</v>
+        <v>61</v>
       </c>
       <c r="B28" s="6">
         <v>5.3</v>
@@ -2790,7 +2790,7 @@
     </row>
     <row r="29" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="B29" s="6">
         <v>17.739999999999998</v>
@@ -2832,7 +2832,7 @@
     </row>
     <row r="30" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B30" s="6">
         <v>5.67</v>
@@ -2879,7 +2879,7 @@
     </row>
     <row r="31" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
-        <v>183</v>
+        <v>80</v>
       </c>
       <c r="B31" s="6">
         <v>4.68</v>
@@ -2921,7 +2921,7 @@
     </row>
     <row r="32" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
-        <v>90</v>
+        <v>44</v>
       </c>
       <c r="B32" s="6">
         <v>9.74</v>
@@ -2963,7 +2963,7 @@
     </row>
     <row r="33" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
-        <v>181</v>
+        <v>79</v>
       </c>
       <c r="B33" s="6">
         <v>2.36</v>
@@ -3005,7 +3005,7 @@
     </row>
     <row r="34" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
-        <v>147</v>
+        <v>68</v>
       </c>
       <c r="B34" s="6">
         <v>8.52</v>
@@ -3047,7 +3047,7 @@
     </row>
     <row r="35" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
-        <v>131</v>
+        <v>60</v>
       </c>
       <c r="B35" s="6">
         <v>8.4</v>
@@ -3094,7 +3094,7 @@
     </row>
     <row r="36" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
-        <v>96</v>
+        <v>47</v>
       </c>
       <c r="B36" s="6">
         <v>4.8600000000000003</v>
@@ -3136,7 +3136,7 @@
     </row>
     <row r="37" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
-        <v>221</v>
+        <v>89</v>
       </c>
       <c r="B37" s="6">
         <v>7.33</v>
@@ -3178,7 +3178,7 @@
     </row>
     <row r="38" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
-        <v>113</v>
+        <v>54</v>
       </c>
       <c r="B38" s="6">
         <v>14.17</v>
@@ -3220,7 +3220,7 @@
     </row>
     <row r="39" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B39" s="6">
         <v>4.87</v>
@@ -3262,7 +3262,7 @@
     </row>
     <row r="40" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
-        <v>180</v>
+        <v>78</v>
       </c>
       <c r="B40" s="8">
         <v>10.029999999999999</v>
@@ -3309,7 +3309,7 @@
     </row>
     <row r="41" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="B41" s="6">
         <v>21.56</v>
@@ -3351,7 +3351,7 @@
     </row>
     <row r="42" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
-        <v>94</v>
+        <v>46</v>
       </c>
       <c r="B42" s="6">
         <v>4.7300000000000004</v>
@@ -3393,7 +3393,7 @@
     </row>
     <row r="43" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A43" s="7" t="s">
-        <v>198</v>
+        <v>82</v>
       </c>
       <c r="B43" s="8">
         <v>10.17</v>
@@ -3435,7 +3435,7 @@
     </row>
     <row r="44" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A44" s="7" t="s">
-        <v>142</v>
+        <v>66</v>
       </c>
       <c r="B44" s="8">
         <v>4.71</v>
@@ -3477,7 +3477,7 @@
     </row>
     <row r="45" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A45" s="7" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B45" s="8">
         <v>5.08</v>
@@ -3524,7 +3524,7 @@
     </row>
     <row r="46" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="B46" s="6">
         <v>2.83</v>
@@ -3566,7 +3566,7 @@
     </row>
     <row r="47" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A47" s="7" t="s">
-        <v>146</v>
+        <v>67</v>
       </c>
       <c r="B47" s="8">
         <v>5.39</v>
@@ -3608,7 +3608,7 @@
     </row>
     <row r="48" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A48" s="7" t="s">
-        <v>128</v>
+        <v>58</v>
       </c>
       <c r="B48" s="8">
         <v>8.2100000000000009</v>
@@ -3650,7 +3650,7 @@
     </row>
     <row r="49" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A49" s="7" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="B49" s="8">
         <v>9.84</v>
@@ -3692,7 +3692,7 @@
     </row>
     <row r="50" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
-        <v>159</v>
+        <v>73</v>
       </c>
       <c r="B50" s="6">
         <v>9.7899999999999991</v>
@@ -3739,7 +3739,7 @@
     </row>
     <row r="51" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A51" s="7" t="s">
-        <v>114</v>
+        <v>55</v>
       </c>
       <c r="B51" s="8">
         <v>7.32</v>
@@ -3781,7 +3781,7 @@
     </row>
     <row r="52" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A52" s="7" t="s">
-        <v>101</v>
+        <v>50</v>
       </c>
       <c r="B52" s="8">
         <v>4.3</v>
@@ -3823,7 +3823,7 @@
     </row>
     <row r="53" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
-        <v>215</v>
+        <v>87</v>
       </c>
       <c r="B53" s="6">
         <v>8</v>
@@ -3865,7 +3865,7 @@
     </row>
     <row r="54" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A54" s="5" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="B54" s="6">
         <v>3.75</v>
@@ -3907,7 +3907,7 @@
     </row>
     <row r="55" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A55" s="7" t="s">
-        <v>140</v>
+        <v>65</v>
       </c>
       <c r="B55" s="8">
         <v>7.79</v>
@@ -3954,7 +3954,7 @@
     </row>
     <row r="56" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A56" s="7" t="s">
-        <v>122</v>
+        <v>57</v>
       </c>
       <c r="B56" s="8">
         <v>5.4</v>
@@ -3996,7 +3996,7 @@
     </row>
     <row r="57" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A57" s="7" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B57" s="8">
         <v>6.88</v>
@@ -4038,7 +4038,7 @@
     </row>
     <row r="58" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A58" s="7" t="s">
-        <v>87</v>
+        <v>43</v>
       </c>
       <c r="B58" s="8">
         <v>10.75</v>
@@ -4080,7 +4080,7 @@
     </row>
     <row r="59" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="B59" s="6">
         <v>4.8099999999999996</v>
@@ -4122,7 +4122,7 @@
     </row>
     <row r="60" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B60" s="6">
         <v>4.1399999999999997</v>
@@ -4164,7 +4164,7 @@
     </row>
     <row r="61" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A61" s="7" t="s">
-        <v>176</v>
+        <v>76</v>
       </c>
       <c r="B61" s="8">
         <v>4.6900000000000004</v>
@@ -4206,7 +4206,7 @@
     </row>
     <row r="62" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
-        <v>129</v>
+        <v>59</v>
       </c>
       <c r="B62" s="6">
         <v>2.92</v>
@@ -4248,7 +4248,7 @@
     </row>
     <row r="63" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B63" s="6">
         <v>8.68</v>
@@ -4290,7 +4290,7 @@
     </row>
     <row r="64" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A64" s="7" t="s">
-        <v>97</v>
+        <v>48</v>
       </c>
       <c r="B64" s="8">
         <v>4.4800000000000004</v>
@@ -4332,7 +4332,7 @@
     </row>
     <row r="65" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A65" s="7" t="s">
-        <v>160</v>
+        <v>74</v>
       </c>
       <c r="B65" s="8">
         <v>10.14</v>
@@ -4374,7 +4374,7 @@
     </row>
     <row r="66" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B66" s="6">
         <v>4.2</v>
@@ -4416,7 +4416,7 @@
     </row>
     <row r="67" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A67" s="5" t="s">
-        <v>153</v>
+        <v>69</v>
       </c>
       <c r="B67" s="6">
         <v>4.47</v>
@@ -4458,7 +4458,7 @@
     </row>
     <row r="68" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
-        <v>102</v>
+        <v>51</v>
       </c>
       <c r="B68" s="6">
         <v>11.44</v>
@@ -4500,7 +4500,7 @@
     </row>
     <row r="69" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A69" s="7" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="B69" s="8">
         <v>6.58</v>
@@ -4542,7 +4542,7 @@
     </row>
     <row r="70" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
-        <v>157</v>
+        <v>72</v>
       </c>
       <c r="B70" s="6">
         <v>22.54</v>
@@ -4584,7 +4584,7 @@
     </row>
     <row r="71" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A71" s="5" t="s">
-        <v>201</v>
+        <v>83</v>
       </c>
       <c r="B71" s="6">
         <v>4.43</v>
@@ -4626,7 +4626,7 @@
     </row>
     <row r="72" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A72" s="7" t="s">
-        <v>105</v>
+        <v>52</v>
       </c>
       <c r="B72" s="8">
         <v>2.36</v>
@@ -4668,7 +4668,7 @@
     </row>
     <row r="73" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A73" s="5" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="B73" s="6">
         <v>4.37</v>
@@ -4710,7 +4710,7 @@
     </row>
     <row r="74" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A74" s="5" t="s">
-        <v>100</v>
+        <v>49</v>
       </c>
       <c r="B74" s="6">
         <v>4.8499999999999996</v>
@@ -4752,7 +4752,7 @@
     </row>
     <row r="75" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A75" s="5" t="s">
-        <v>217</v>
+        <v>88</v>
       </c>
       <c r="B75" s="6">
         <v>4</v>
@@ -4794,7 +4794,7 @@
     </row>
     <row r="76" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A76" s="7" t="s">
-        <v>204</v>
+        <v>84</v>
       </c>
       <c r="B76" s="8">
         <v>3.26</v>
@@ -4836,7 +4836,7 @@
     </row>
     <row r="77" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A77" s="7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B77" s="8">
         <v>6.43</v>
@@ -4878,7 +4878,7 @@
     </row>
     <row r="78" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
-        <v>137</v>
+        <v>63</v>
       </c>
       <c r="B78" s="6">
         <v>19.14</v>
@@ -4920,7 +4920,7 @@
     </row>
     <row r="79" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A79" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B79" s="6">
         <v>6.11</v>
@@ -4962,7 +4962,7 @@
     </row>
     <row r="80" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
-        <v>155</v>
+        <v>70</v>
       </c>
       <c r="B80" s="6">
         <v>4.43</v>
@@ -5004,7 +5004,7 @@
     </row>
     <row r="81" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A81" s="5" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="B81" s="6">
         <v>2.4</v>
@@ -5046,7 +5046,7 @@
     </row>
     <row r="82" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A82" s="7" t="s">
-        <v>120</v>
+        <v>56</v>
       </c>
       <c r="B82" s="8">
         <v>2.75</v>
@@ -5088,7 +5088,7 @@
     </row>
     <row r="83" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A83" s="7" t="s">
-        <v>170</v>
+        <v>75</v>
       </c>
       <c r="B83" s="8">
         <v>4.0599999999999996</v>
@@ -5130,7 +5130,7 @@
     </row>
     <row r="84" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
-        <v>205</v>
+        <v>85</v>
       </c>
       <c r="B84" s="6">
         <v>5.83</v>
@@ -5172,7 +5172,7 @@
     </row>
     <row r="85" spans="1:22" ht="15.6" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A85" s="16" t="s">
-        <v>206</v>
+        <v>86</v>
       </c>
       <c r="B85" s="17">
         <v>3.35</v>
@@ -5214,7 +5214,7 @@
     </row>
     <row r="86" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A86" s="14" t="s">
-        <v>106</v>
+        <v>164</v>
       </c>
       <c r="B86" s="15">
         <v>8.9</v>
@@ -5256,7 +5256,7 @@
     </row>
     <row r="87" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A87" s="7" t="s">
-        <v>29</v>
+        <v>165</v>
       </c>
       <c r="B87" s="8">
         <v>8.2899999999999991</v>
@@ -5298,7 +5298,7 @@
     </row>
     <row r="88" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A88" s="5" t="s">
-        <v>119</v>
+        <v>166</v>
       </c>
       <c r="B88" s="6">
         <v>6.76</v>
@@ -5340,7 +5340,7 @@
     </row>
     <row r="89" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A89" s="7" t="s">
-        <v>132</v>
+        <v>167</v>
       </c>
       <c r="B89" s="8">
         <v>4.7699999999999996</v>
@@ -5382,7 +5382,7 @@
     </row>
     <row r="90" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A90" s="7" t="s">
-        <v>218</v>
+        <v>168</v>
       </c>
       <c r="B90" s="8">
         <v>4.67</v>
@@ -5424,7 +5424,7 @@
     </row>
     <row r="91" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A91" s="7" t="s">
-        <v>89</v>
+        <v>169</v>
       </c>
       <c r="B91" s="8">
         <v>5.75</v>
@@ -5466,7 +5466,7 @@
     </row>
     <row r="92" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A92" s="5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B92" s="6">
         <v>5.41</v>
@@ -5508,7 +5508,7 @@
     </row>
     <row r="93" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A93" s="5" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="B93" s="6">
         <v>9.9499999999999993</v>
@@ -5550,7 +5550,7 @@
     </row>
     <row r="94" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A94" s="7" t="s">
-        <v>107</v>
+        <v>172</v>
       </c>
       <c r="B94" s="8">
         <v>5.01</v>
@@ -5592,7 +5592,7 @@
     </row>
     <row r="95" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A95" s="5" t="s">
-        <v>141</v>
+        <v>173</v>
       </c>
       <c r="B95" s="6">
         <v>5.3</v>
@@ -5634,7 +5634,7 @@
     </row>
     <row r="96" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A96" s="5" t="s">
-        <v>56</v>
+        <v>174</v>
       </c>
       <c r="B96" s="6">
         <v>17.739999999999998</v>
@@ -5676,7 +5676,7 @@
     </row>
     <row r="97" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A97" s="7" t="s">
-        <v>73</v>
+        <v>175</v>
       </c>
       <c r="B97" s="8">
         <v>5.8</v>
@@ -5718,7 +5718,7 @@
     </row>
     <row r="98" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A98" s="5" t="s">
-        <v>62</v>
+        <v>176</v>
       </c>
       <c r="B98" s="6">
         <v>4.68</v>
@@ -5760,7 +5760,7 @@
     </row>
     <row r="99" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A99" s="7" t="s">
-        <v>75</v>
+        <v>177</v>
       </c>
       <c r="B99" s="8">
         <v>9.81</v>
@@ -5802,7 +5802,7 @@
     </row>
     <row r="100" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A100" s="7" t="s">
-        <v>53</v>
+        <v>178</v>
       </c>
       <c r="B100" s="8">
         <v>2.36</v>
@@ -5844,7 +5844,7 @@
     </row>
     <row r="101" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A101" s="7" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="B101" s="8">
         <v>8.51</v>
@@ -5886,7 +5886,7 @@
     </row>
     <row r="102" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A102" s="5" t="s">
-        <v>213</v>
+        <v>180</v>
       </c>
       <c r="B102" s="6">
         <v>8.56</v>
@@ -5928,7 +5928,7 @@
     </row>
     <row r="103" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A103" s="7" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="B103" s="8">
         <v>4.8600000000000003</v>
@@ -5970,7 +5970,7 @@
     </row>
     <row r="104" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A104" s="5" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="B104" s="6">
         <v>7.33</v>
@@ -6012,7 +6012,7 @@
     </row>
     <row r="105" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A105" s="5" t="s">
-        <v>78</v>
+        <v>183</v>
       </c>
       <c r="B105" s="6">
         <v>14.2</v>
@@ -6054,7 +6054,7 @@
     </row>
     <row r="106" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A106" s="5" t="s">
-        <v>40</v>
+        <v>184</v>
       </c>
       <c r="B106" s="6">
         <v>4.76</v>
@@ -6096,7 +6096,7 @@
     </row>
     <row r="107" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A107" s="5" t="s">
-        <v>223</v>
+        <v>185</v>
       </c>
       <c r="B107" s="6">
         <v>10.029999999999999</v>
@@ -6138,7 +6138,7 @@
     </row>
     <row r="108" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A108" s="5" t="s">
-        <v>121</v>
+        <v>186</v>
       </c>
       <c r="B108" s="6">
         <v>21.5</v>
@@ -6180,7 +6180,7 @@
     </row>
     <row r="109" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A109" s="7" t="s">
-        <v>27</v>
+        <v>187</v>
       </c>
       <c r="B109" s="8">
         <v>4.7300000000000004</v>
@@ -6222,7 +6222,7 @@
     </row>
     <row r="110" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A110" s="5" t="s">
-        <v>139</v>
+        <v>188</v>
       </c>
       <c r="B110" s="6">
         <v>10.17</v>
@@ -6264,7 +6264,7 @@
     </row>
     <row r="111" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A111" s="7" t="s">
-        <v>59</v>
+        <v>189</v>
       </c>
       <c r="B111" s="8">
         <v>4.5599999999999996</v>
@@ -6306,7 +6306,7 @@
     </row>
     <row r="112" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A112" s="7" t="s">
-        <v>63</v>
+        <v>190</v>
       </c>
       <c r="B112" s="8">
         <v>5.08</v>
@@ -6348,7 +6348,7 @@
     </row>
     <row r="113" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A113" s="7" t="s">
-        <v>134</v>
+        <v>191</v>
       </c>
       <c r="B113" s="8">
         <v>2.83</v>
@@ -6390,7 +6390,7 @@
     </row>
     <row r="114" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A114" s="5" t="s">
-        <v>98</v>
+        <v>192</v>
       </c>
       <c r="B114" s="6">
         <v>5.39</v>
@@ -6432,7 +6432,7 @@
     </row>
     <row r="115" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A115" s="7" t="s">
-        <v>25</v>
+        <v>193</v>
       </c>
       <c r="B115" s="8">
         <v>8.26</v>
@@ -6474,7 +6474,7 @@
     </row>
     <row r="116" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A116" s="7" t="s">
-        <v>182</v>
+        <v>194</v>
       </c>
       <c r="B116" s="8">
         <v>9.9499999999999993</v>
@@ -6516,7 +6516,7 @@
     </row>
     <row r="117" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A117" s="5" t="s">
-        <v>108</v>
+        <v>195</v>
       </c>
       <c r="B117" s="6">
         <v>9.93</v>
@@ -6558,7 +6558,7 @@
     </row>
     <row r="118" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A118" s="5" t="s">
-        <v>143</v>
+        <v>196</v>
       </c>
       <c r="B118" s="6">
         <v>7.38</v>
@@ -6600,7 +6600,7 @@
     </row>
     <row r="119" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A119" s="7" t="s">
-        <v>103</v>
+        <v>197</v>
       </c>
       <c r="B119" s="8">
         <v>4.32</v>
@@ -6642,7 +6642,7 @@
     </row>
     <row r="120" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A120" s="5" t="s">
-        <v>80</v>
+        <v>198</v>
       </c>
       <c r="B120" s="6">
         <v>8.14</v>
@@ -6684,7 +6684,7 @@
     </row>
     <row r="121" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A121" s="7" t="s">
-        <v>49</v>
+        <v>199</v>
       </c>
       <c r="B121" s="8">
         <v>3.83</v>
@@ -6726,7 +6726,7 @@
     </row>
     <row r="122" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A122" s="7" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="B122" s="8">
         <v>7.79</v>
@@ -6768,7 +6768,7 @@
     </row>
     <row r="123" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A123" s="5" t="s">
-        <v>169</v>
+        <v>201</v>
       </c>
       <c r="B123" s="6">
         <v>5.4</v>
@@ -6810,7 +6810,7 @@
     </row>
     <row r="124" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A124" s="5" t="s">
-        <v>145</v>
+        <v>202</v>
       </c>
       <c r="B124" s="6">
         <v>6.88</v>
@@ -6852,7 +6852,7 @@
     </row>
     <row r="125" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A125" s="5" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="B125" s="6">
         <v>11</v>
@@ -6894,7 +6894,7 @@
     </row>
     <row r="126" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A126" s="5" t="s">
-        <v>76</v>
+        <v>204</v>
       </c>
       <c r="B126" s="6">
         <v>4.8099999999999996</v>
@@ -6936,7 +6936,7 @@
     </row>
     <row r="127" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A127" s="7" t="s">
-        <v>57</v>
+        <v>205</v>
       </c>
       <c r="B127" s="8">
         <v>4.1399999999999997</v>
@@ -6978,7 +6978,7 @@
     </row>
     <row r="128" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A128" s="5" t="s">
-        <v>163</v>
+        <v>206</v>
       </c>
       <c r="B128" s="6">
         <v>4.6900000000000004</v>
@@ -7020,7 +7020,7 @@
     </row>
     <row r="129" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A129" s="7" t="s">
-        <v>24</v>
+        <v>207</v>
       </c>
       <c r="B129" s="8">
         <v>2.92</v>
@@ -7062,7 +7062,7 @@
     </row>
     <row r="130" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A130" s="5" t="s">
-        <v>123</v>
+        <v>208</v>
       </c>
       <c r="B130" s="6">
         <v>8.73</v>
@@ -7104,7 +7104,7 @@
     </row>
     <row r="131" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A131" s="7" t="s">
-        <v>41</v>
+        <v>209</v>
       </c>
       <c r="B131" s="8">
         <v>4.4800000000000004</v>
@@ -7146,7 +7146,7 @@
     </row>
     <row r="132" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A132" s="5" t="s">
-        <v>127</v>
+        <v>210</v>
       </c>
       <c r="B132" s="6">
         <v>9.7100000000000009</v>
@@ -7188,7 +7188,7 @@
     </row>
     <row r="133" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A133" s="7" t="s">
-        <v>116</v>
+        <v>211</v>
       </c>
       <c r="B133" s="8">
         <v>4.26</v>
@@ -7230,7 +7230,7 @@
     </row>
     <row r="134" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A134" s="5" t="s">
-        <v>175</v>
+        <v>212</v>
       </c>
       <c r="B134" s="6">
         <v>4.13</v>
@@ -7272,7 +7272,7 @@
     </row>
     <row r="135" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A135" s="7" t="s">
-        <v>51</v>
+        <v>213</v>
       </c>
       <c r="B135" s="8">
         <v>11.44</v>
@@ -7314,7 +7314,7 @@
     </row>
     <row r="136" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A136" s="7" t="s">
-        <v>126</v>
+        <v>214</v>
       </c>
       <c r="B136" s="8">
         <v>6.58</v>
@@ -7356,7 +7356,7 @@
     </row>
     <row r="137" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A137" s="7" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B137" s="8">
         <v>22.54</v>
@@ -7398,7 +7398,7 @@
     </row>
     <row r="138" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A138" s="5" t="s">
-        <v>203</v>
+        <v>216</v>
       </c>
       <c r="B138" s="6">
         <v>4.43</v>
@@ -7440,7 +7440,7 @@
     </row>
     <row r="139" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A139" s="7" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="B139" s="8">
         <v>2.36</v>
@@ -7482,7 +7482,7 @@
     </row>
     <row r="140" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A140" s="7" t="s">
-        <v>164</v>
+        <v>218</v>
       </c>
       <c r="B140" s="8">
         <v>4.16</v>
@@ -7524,7 +7524,7 @@
     </row>
     <row r="141" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A141" s="7" t="s">
-        <v>55</v>
+        <v>219</v>
       </c>
       <c r="B141" s="8">
         <v>4.8499999999999996</v>
@@ -7566,7 +7566,7 @@
     </row>
     <row r="142" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A142" s="7" t="s">
-        <v>112</v>
+        <v>220</v>
       </c>
       <c r="B142" s="8">
         <v>4</v>
@@ -7608,7 +7608,7 @@
     </row>
     <row r="143" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A143" s="7" t="s">
-        <v>196</v>
+        <v>221</v>
       </c>
       <c r="B143" s="8">
         <v>3.17</v>
@@ -7650,7 +7650,7 @@
     </row>
     <row r="144" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A144" s="5" t="s">
-        <v>115</v>
+        <v>222</v>
       </c>
       <c r="B144" s="6">
         <v>6.43</v>
@@ -7692,7 +7692,7 @@
     </row>
     <row r="145" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A145" s="5" t="s">
-        <v>197</v>
+        <v>223</v>
       </c>
       <c r="B145" s="6">
         <v>19.14</v>
@@ -7734,7 +7734,7 @@
     </row>
     <row r="146" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A146" s="5" t="s">
-        <v>110</v>
+        <v>224</v>
       </c>
       <c r="B146" s="6">
         <v>6.11</v>
@@ -7776,7 +7776,7 @@
     </row>
     <row r="147" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A147" s="5" t="s">
-        <v>44</v>
+        <v>225</v>
       </c>
       <c r="B147" s="6">
         <v>4.43</v>
@@ -7818,7 +7818,7 @@
     </row>
     <row r="148" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A148" s="5" t="s">
-        <v>26</v>
+        <v>226</v>
       </c>
       <c r="B148" s="6">
         <v>2.8</v>
@@ -7860,7 +7860,7 @@
     </row>
     <row r="149" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A149" s="5" t="s">
-        <v>88</v>
+        <v>227</v>
       </c>
       <c r="B149" s="6">
         <v>2.75</v>
@@ -7902,7 +7902,7 @@
     </row>
     <row r="150" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A150" s="5" t="s">
-        <v>64</v>
+        <v>228</v>
       </c>
       <c r="B150" s="6">
         <v>4.1900000000000004</v>
@@ -7944,7 +7944,7 @@
     </row>
     <row r="151" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A151" s="5" t="s">
-        <v>84</v>
+        <v>229</v>
       </c>
       <c r="B151" s="6">
         <v>5.83</v>
@@ -7986,7 +7986,7 @@
     </row>
     <row r="152" spans="1:22" ht="15.6" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A152" s="16" t="s">
-        <v>166</v>
+        <v>230</v>
       </c>
       <c r="B152" s="17">
         <v>3.35</v>
@@ -8028,7 +8028,7 @@
     </row>
     <row r="153" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A153" s="14" t="s">
-        <v>161</v>
+        <v>97</v>
       </c>
       <c r="B153" s="15">
         <v>8.9</v>
@@ -8070,7 +8070,7 @@
     </row>
     <row r="154" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A154" s="7" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
       <c r="B154" s="8">
         <v>8.33</v>
@@ -8112,7 +8112,7 @@
     </row>
     <row r="155" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A155" s="5" t="s">
-        <v>133</v>
+        <v>99</v>
       </c>
       <c r="B155" s="6">
         <v>6.38</v>
@@ -8154,7 +8154,7 @@
     </row>
     <row r="156" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A156" s="7" t="s">
-        <v>37</v>
+        <v>100</v>
       </c>
       <c r="B156" s="8">
         <v>4.7699999999999996</v>
@@ -8196,7 +8196,7 @@
     </row>
     <row r="157" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A157" s="7" t="s">
-        <v>148</v>
+        <v>101</v>
       </c>
       <c r="B157" s="8">
         <v>4.67</v>
@@ -8238,7 +8238,7 @@
     </row>
     <row r="158" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A158" s="5" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
       <c r="B158" s="6">
         <v>5.75</v>
@@ -8280,7 +8280,7 @@
     </row>
     <row r="159" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A159" s="7" t="s">
-        <v>208</v>
+        <v>103</v>
       </c>
       <c r="B159" s="8">
         <v>5.41</v>
@@ -8322,7 +8322,7 @@
     </row>
     <row r="160" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A160" s="7" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="B160" s="8">
         <v>10.24</v>
@@ -8364,7 +8364,7 @@
     </row>
     <row r="161" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A161" s="5" t="s">
-        <v>199</v>
+        <v>105</v>
       </c>
       <c r="B161" s="6">
         <v>5.01</v>
@@ -8406,7 +8406,7 @@
     </row>
     <row r="162" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A162" s="7" t="s">
-        <v>83</v>
+        <v>106</v>
       </c>
       <c r="B162" s="8">
         <v>5.3</v>
@@ -8448,7 +8448,7 @@
     </row>
     <row r="163" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A163" s="5" t="s">
-        <v>151</v>
+        <v>107</v>
       </c>
       <c r="B163" s="6">
         <v>17.739999999999998</v>
@@ -8490,7 +8490,7 @@
     </row>
     <row r="164" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A164" s="5" t="s">
-        <v>187</v>
+        <v>108</v>
       </c>
       <c r="B164" s="6">
         <v>5.8</v>
@@ -8532,7 +8532,7 @@
     </row>
     <row r="165" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A165" s="7" t="s">
-        <v>69</v>
+        <v>109</v>
       </c>
       <c r="B165" s="8">
         <v>4.68</v>
@@ -8574,7 +8574,7 @@
     </row>
     <row r="166" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A166" s="7" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="B166" s="8">
         <v>9.81</v>
@@ -8616,7 +8616,7 @@
     </row>
     <row r="167" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A167" s="5" t="s">
-        <v>171</v>
+        <v>111</v>
       </c>
       <c r="B167" s="6">
         <v>2.36</v>
@@ -8658,7 +8658,7 @@
     </row>
     <row r="168" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A168" s="7" t="s">
-        <v>200</v>
+        <v>112</v>
       </c>
       <c r="B168" s="8">
         <v>8.52</v>
@@ -8700,7 +8700,7 @@
     </row>
     <row r="169" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A169" s="5" t="s">
-        <v>165</v>
+        <v>113</v>
       </c>
       <c r="B169" s="6">
         <v>8.4</v>
@@ -8742,7 +8742,7 @@
     </row>
     <row r="170" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A170" s="7" t="s">
-        <v>81</v>
+        <v>114</v>
       </c>
       <c r="B170" s="8">
         <v>4.8600000000000003</v>
@@ -8784,7 +8784,7 @@
     </row>
     <row r="171" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A171" s="5" t="s">
-        <v>82</v>
+        <v>115</v>
       </c>
       <c r="B171" s="6">
         <v>7.33</v>
@@ -8826,7 +8826,7 @@
     </row>
     <row r="172" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A172" s="5" t="s">
-        <v>211</v>
+        <v>116</v>
       </c>
       <c r="B172" s="6">
         <v>14.19</v>
@@ -8868,7 +8868,7 @@
     </row>
     <row r="173" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A173" s="7" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
       <c r="B173" s="8">
         <v>4.87</v>
@@ -8910,7 +8910,7 @@
     </row>
     <row r="174" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A174" s="7" t="s">
-        <v>39</v>
+        <v>118</v>
       </c>
       <c r="B174" s="8">
         <v>10.029999999999999</v>
@@ -8952,7 +8952,7 @@
     </row>
     <row r="175" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A175" s="7" t="s">
-        <v>43</v>
+        <v>119</v>
       </c>
       <c r="B175" s="8">
         <v>21.59</v>
@@ -8994,7 +8994,7 @@
     </row>
     <row r="176" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A176" s="5" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="B176" s="6">
         <v>4.7300000000000004</v>
@@ -9036,7 +9036,7 @@
     </row>
     <row r="177" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A177" s="7" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B177" s="8">
         <v>10.17</v>
@@ -9078,7 +9078,7 @@
     </row>
     <row r="178" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A178" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B178" s="8">
         <v>4.71</v>
@@ -9120,7 +9120,7 @@
     </row>
     <row r="179" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A179" s="7" t="s">
-        <v>172</v>
+        <v>123</v>
       </c>
       <c r="B179" s="8">
         <v>5.08</v>
@@ -9162,7 +9162,7 @@
     </row>
     <row r="180" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A180" s="5" t="s">
-        <v>68</v>
+        <v>124</v>
       </c>
       <c r="B180" s="6">
         <v>2.83</v>
@@ -9204,7 +9204,7 @@
     </row>
     <row r="181" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A181" s="7" t="s">
-        <v>174</v>
+        <v>125</v>
       </c>
       <c r="B181" s="8">
         <v>5.41</v>
@@ -9246,7 +9246,7 @@
     </row>
     <row r="182" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A182" s="7" t="s">
-        <v>85</v>
+        <v>126</v>
       </c>
       <c r="B182" s="8">
         <v>8.26</v>
@@ -9288,7 +9288,7 @@
     </row>
     <row r="183" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A183" s="7" t="s">
-        <v>188</v>
+        <v>127</v>
       </c>
       <c r="B183" s="8">
         <v>9.9499999999999993</v>
@@ -9330,7 +9330,7 @@
     </row>
     <row r="184" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A184" s="5" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="B184" s="6">
         <v>9.93</v>
@@ -9372,7 +9372,7 @@
     </row>
     <row r="185" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A185" s="7" t="s">
-        <v>162</v>
+        <v>129</v>
       </c>
       <c r="B185" s="8">
         <v>7.38</v>
@@ -9414,7 +9414,7 @@
     </row>
     <row r="186" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A186" s="5" t="s">
-        <v>23</v>
+        <v>130</v>
       </c>
       <c r="B186" s="6">
         <v>4.32</v>
@@ -9456,7 +9456,7 @@
     </row>
     <row r="187" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A187" s="7" t="s">
-        <v>216</v>
+        <v>131</v>
       </c>
       <c r="B187" s="8">
         <v>8.14</v>
@@ -9498,7 +9498,7 @@
     </row>
     <row r="188" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A188" s="5" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="B188" s="6">
         <v>3.83</v>
@@ -9540,7 +9540,7 @@
     </row>
     <row r="189" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A189" s="7" t="s">
-        <v>214</v>
+        <v>133</v>
       </c>
       <c r="B189" s="8">
         <v>7.79</v>
@@ -9582,7 +9582,7 @@
     </row>
     <row r="190" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A190" s="5" t="s">
-        <v>219</v>
+        <v>134</v>
       </c>
       <c r="B190" s="6">
         <v>5.4</v>
@@ -9624,7 +9624,7 @@
     </row>
     <row r="191" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A191" s="7" t="s">
-        <v>190</v>
+        <v>135</v>
       </c>
       <c r="B191" s="8">
         <v>6.88</v>
@@ -9666,7 +9666,7 @@
     </row>
     <row r="192" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A192" s="5" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="B192" s="6">
         <v>11</v>
@@ -9708,7 +9708,7 @@
     </row>
     <row r="193" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A193" s="5" t="s">
-        <v>86</v>
+        <v>137</v>
       </c>
       <c r="B193" s="6">
         <v>4.8099999999999996</v>
@@ -9750,7 +9750,7 @@
     </row>
     <row r="194" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A194" s="7" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B194" s="8">
         <v>4.1399999999999997</v>
@@ -9792,7 +9792,7 @@
     </row>
     <row r="195" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A195" s="7" t="s">
-        <v>220</v>
+        <v>139</v>
       </c>
       <c r="B195" s="8">
         <v>4.6900000000000004</v>
@@ -9834,7 +9834,7 @@
     </row>
     <row r="196" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A196" s="7" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="B196" s="8">
         <v>2.92</v>
@@ -9876,7 +9876,7 @@
     </row>
     <row r="197" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A197" s="5" t="s">
-        <v>167</v>
+        <v>141</v>
       </c>
       <c r="B197" s="6">
         <v>8.73</v>
@@ -9918,7 +9918,7 @@
     </row>
     <row r="198" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A198" s="7" t="s">
-        <v>184</v>
+        <v>142</v>
       </c>
       <c r="B198" s="8">
         <v>4.4800000000000004</v>
@@ -9960,7 +9960,7 @@
     </row>
     <row r="199" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A199" s="5" t="s">
-        <v>189</v>
+        <v>143</v>
       </c>
       <c r="B199" s="6">
         <v>10</v>
@@ -10002,7 +10002,7 @@
     </row>
     <row r="200" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A200" s="5" t="s">
-        <v>195</v>
+        <v>144</v>
       </c>
       <c r="B200" s="6">
         <v>4.26</v>
@@ -10044,7 +10044,7 @@
     </row>
     <row r="201" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A201" s="5" t="s">
-        <v>209</v>
+        <v>145</v>
       </c>
       <c r="B201" s="6">
         <v>4.47</v>
@@ -10086,7 +10086,7 @@
     </row>
     <row r="202" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A202" s="7" t="s">
-        <v>45</v>
+        <v>146</v>
       </c>
       <c r="B202" s="8">
         <v>11.44</v>
@@ -10128,7 +10128,7 @@
     </row>
     <row r="203" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A203" s="7" t="s">
-        <v>222</v>
+        <v>147</v>
       </c>
       <c r="B203" s="8">
         <v>6.58</v>
@@ -10170,7 +10170,7 @@
     </row>
     <row r="204" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A204" s="7" t="s">
-        <v>33</v>
+        <v>148</v>
       </c>
       <c r="B204" s="8">
         <v>22.54</v>
@@ -10212,7 +10212,7 @@
     </row>
     <row r="205" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A205" s="7" t="s">
-        <v>202</v>
+        <v>149</v>
       </c>
       <c r="B205" s="8">
         <v>4.43</v>
@@ -10254,7 +10254,7 @@
     </row>
     <row r="206" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A206" s="5" t="s">
-        <v>34</v>
+        <v>150</v>
       </c>
       <c r="B206" s="6">
         <v>2.5499999999999998</v>
@@ -10296,7 +10296,7 @@
     </row>
     <row r="207" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A207" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B207" s="8">
         <v>4.37</v>
@@ -10338,7 +10338,7 @@
     </row>
     <row r="208" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A208" s="5" t="s">
-        <v>60</v>
+        <v>152</v>
       </c>
       <c r="B208" s="6">
         <v>4.8499999999999996</v>
@@ -10380,7 +10380,7 @@
     </row>
     <row r="209" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A209" s="7" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B209" s="8">
         <v>4</v>
@@ -10422,7 +10422,7 @@
     </row>
     <row r="210" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A210" s="5" t="s">
-        <v>207</v>
+        <v>154</v>
       </c>
       <c r="B210" s="6">
         <v>3.26</v>
@@ -10464,7 +10464,7 @@
     </row>
     <row r="211" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A211" s="7" t="s">
-        <v>192</v>
+        <v>155</v>
       </c>
       <c r="B211" s="8">
         <v>6.43</v>
@@ -10506,7 +10506,7 @@
     </row>
     <row r="212" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A212" s="7" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B212" s="8">
         <v>19.14</v>
@@ -10548,7 +10548,7 @@
     </row>
     <row r="213" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A213" s="7" t="s">
-        <v>77</v>
+        <v>157</v>
       </c>
       <c r="B213" s="8">
         <v>6.11</v>
@@ -10590,7 +10590,7 @@
     </row>
     <row r="214" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A214" s="7" t="s">
-        <v>111</v>
+        <v>158</v>
       </c>
       <c r="B214" s="8">
         <v>4.43</v>
@@ -10632,7 +10632,7 @@
     </row>
     <row r="215" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A215" s="5" t="s">
-        <v>70</v>
+        <v>159</v>
       </c>
       <c r="B215" s="6">
         <v>2.8</v>
@@ -10674,7 +10674,7 @@
     </row>
     <row r="216" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A216" s="7" t="s">
-        <v>79</v>
+        <v>160</v>
       </c>
       <c r="B216" s="8">
         <v>3</v>
@@ -10716,7 +10716,7 @@
     </row>
     <row r="217" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A217" s="7" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
       <c r="B217" s="8">
         <v>4.1900000000000004</v>
@@ -10758,7 +10758,7 @@
     </row>
     <row r="218" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A218" s="7" t="s">
-        <v>65</v>
+        <v>162</v>
       </c>
       <c r="B218" s="8">
         <v>5.83</v>
@@ -10800,7 +10800,7 @@
     </row>
     <row r="219" spans="1:22" ht="15" x14ac:dyDescent="0.35">
       <c r="A219" s="7" t="s">
-        <v>93</v>
+        <v>163</v>
       </c>
       <c r="B219" s="8">
         <v>3.35</v>
@@ -10842,7 +10842,7 @@
     </row>
     <row r="220" spans="1:22" ht="28.8" x14ac:dyDescent="0.35">
       <c r="A220" s="12" t="s">
-        <v>230</v>
+        <v>96</v>
       </c>
       <c r="B220" s="12" t="s">
         <v>15</v>
@@ -10884,7 +10884,7 @@
     </row>
     <row r="221" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A221" s="11" t="s">
-        <v>225</v>
+        <v>91</v>
       </c>
       <c r="B221" s="18">
         <f>SUM(B19:B219)</f>
@@ -10923,7 +10923,7 @@
     </row>
     <row r="222" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A222" s="11" t="s">
-        <v>227</v>
+        <v>93</v>
       </c>
       <c r="B222" s="19">
         <f>AVERAGE(B19:B219)</f>
@@ -10962,7 +10962,7 @@
     </row>
     <row r="223" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A223" s="9" t="s">
-        <v>226</v>
+        <v>92</v>
       </c>
       <c r="B223" s="18">
         <f>MIN(B19:B219)</f>
@@ -11001,7 +11001,7 @@
     </row>
     <row r="224" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A224" s="9" t="s">
-        <v>228</v>
+        <v>94</v>
       </c>
       <c r="B224" s="19">
         <f>MAX(B19:B219)</f>
@@ -11040,7 +11040,7 @@
     </row>
     <row r="225" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A225" s="9" t="s">
-        <v>224</v>
+        <v>90</v>
       </c>
       <c r="B225" s="18">
         <f>_xlfn.STDEV.S(B19:B219)</f>
@@ -11079,7 +11079,7 @@
     </row>
     <row r="226" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A226" s="11" t="s">
-        <v>229</v>
+        <v>95</v>
       </c>
       <c r="B226" s="19">
         <f>_xlfn.VAR.S(B19:B219)</f>

</xml_diff>